<commit_message>
Added analytics and data processing pipelines
</commit_message>
<xml_diff>
--- a/data/alibaba/alibaba_02072022.xlsx
+++ b/data/alibaba/alibaba_02072022.xlsx
@@ -2758,7 +2758,7 @@
     <t>You will be a key member of GSA (Global Strategic Accounts) Regional Payment Operations Centre to help achieve the company's global vision. We are aiming to provide the best payment experience to Ant's global strategic partners. As the business solution manager of new and existing accounts, you will be establishing a strong relationship with Ant's global strategic partners, helping them to define co-create scalable e-wallet and / or payment solutions &amp; products, all with the goal to help our partners achieve their business goals. - Function as a business solution expert to present our products and value proposition in business development engagement with merchants. - Responsible for identifying good matches between merchant’s requirements and our e-wallet and payment product baseline, building business cases for merchant acquisition, driving the solutioning for possible gaps with PD, seeking approval for the solutions from compliance and prioritizing tech resources for implementation for new and existing accounts. - Responsible for defining and improving SOP for newly acquired merchants or newly established business service to ensure the optimal operation efficiency. - Take measures to address regulatory concerns and ensure business operations and product offering adhere to the ever-changing requirements of the regulator. - Manage internal and external stakeholders including preparing and providing periodic updates to them on the payments business - Translate local insights and trends to product features that enhance our product competitiveness.</t>
   </si>
   <si>
-    <t>· Daily responsibilities on entities wise transactional and account level reconciliation on banks and acquirers, investigate and resolve on settlement discrepancies, working closely with customer service on case handling, other supporting functions including but not limited to chargeback, refund, and wallet withdrawal · Daily monitoring on incoming fund and ensuring sufficient liquidity, on time settlement and remittance to merchants, compliance to safeguarding requirement · Proper documentation of the responsible entities’ process and SOP, monthly reporting or whenever required to on regulatory, financial, MDR and CFTB · Review and align on the operational process, perform analysis and identify area of improvement on system enhancement, process excellence, revise SOP etc. ensuring operation is compliance with country regulation · Cross departments collaboration with business, technology, product and so on to support new project and new channel going LIVE</t>
+    <t>- Daily responsibilities on entities wise transactional and account level reconciliation on banks and acquirers, investigate and resolve on settlement discrepancies, working closely with customer service on case handling, other supporting functions including but not limited to chargeback, refund, and wallet withdrawal - Daily monitoring on incoming fund and ensuring sufficient liquidity, on time settlement and remittance to merchants, compliance to safeguarding requirement - Proper documentation of the responsible entities’ process and SOP, monthly reporting or whenever required to on regulatory, financial, MDR and CFTB - Review and align on the operational process, perform analysis and identify area of improvement on system enhancement, process excellence, revise SOP etc. ensuring operation is compliance with country regulation - Cross departments collaboration with business, technology, product and so on to support new project and new channel going LIVE</t>
   </si>
   <si>
     <t>1. 负责仓库流程体系建设，推动流程变革优化，提高仓储、配送效率，降低成本。 2. 负责仓库运营管理，负责制定仓配各项KPI指标，并推动达到预期目标。 3. 管控仓库的发货准确率、及时率，库存准确、效期安全及配送及时，避免客户投诉，提升客户满意度。 4. 负责对仓库仓配日常作业进行检查、监督、提案改善，保障仓配日常操作顺畅。 5. 负责与公司业务前端协同，根据公司业务发展计划对仓配布局及时作调整以满足公司业务发展需求。 6. 完成部门领导安排的其他相关工作。</t>
@@ -2920,7 +2920,7 @@
     <t>As the AML management team member, the senior manager serves as the key management staff supporting the Head of AML, providing critical coverage across namely policy and governance. The incumbent will have oversight and responsibility for: 1. Policy – to ensure that the right AML and sanctions and other relevant policies and procedures such as customer risk assessment, Institution Risk Assessment methodologies are formulated and put in place for International Group and its entities, and promote awareness. This position is required to: a)work closely with Group entities to formulate, implement Group wide AML, sanctions and other relevant policies and procedures; b)identify changes in laws and regulations which impact the firm’s AML, sanctions and other relevant policies and procedures and timely update the Group policies and procedures; c)provide guidance and training to Group and its entities and business units on implementation of policies and procedures, and how to comply with the relevant laws and regulations. 2. Governance – to build and strengthen the governance oversight and enable the function to efficiently manage Business-As-Usual and also projects. This position is required to: a)proactively manage all the issues owned by the function to ensure that the actions are in line with Group’s standards and direction; b)lead key processes such as organising governance committees, governance reporting, including reporting to senior management committees of the firm; c)handle, challenge and oversee all strategic initiatives and ensure that they align with the standards, policies and procedures; d)enhance strategic planning and governance which support International business units and entities.</t>
   </si>
   <si>
-    <t>You will be a key member of Ant Group international product team to help achieve company’s global vision. You will design and execute the development and integration of world-class payment capabilities to strategic e-commerce platforms, empowering commerce-payment ecosystem in overseas emerging markets. You will take ownership of the products to ensure optimal user experience, operation efficiency, security and compliant to regulations. Responsibilities: · Play the role as a key product manager of digital wallet product which covers user acquisition, KYC / verification, top up / payment, promotion and every expects of a typical digital wallet service · Closely collaborate with strategic e-commerce platforms and other partners. Deliver and manage product solutions that help achieve business goals. · Articulate value propositions of business initiatives. Translate business requirements into product requirement that is concrete and clear for the development team to work on. · Understand competitive landscape in local markets, discover market insights and identify customer pain points · Take ownership of the product, manage short / long term product roadmap based on the business and customer value · Collaborate with different teams and stakeholders, project-manage and oversee E2E development process. · Understand user mindset and behavior through research, observation, data-analysis and E2E testing. Engineer and deliver frictionless and relevant digital wallet / payment experience to customers. · Act as an ambassador for the product internally and externally, and as the primary product contact for queries related to the product. · Understand, define and track product performance metric. Consistently iterate the products based on analysis of the product performance metric · Off-hour and on-site support to ensure product integrity during high traffic events</t>
+    <t>You will be a key member of Ant Group international product team to help achieve company’s global vision. You will design and execute the development and integration of world-class payment capabilities to strategic e-commerce platforms, empowering commerce-payment ecosystem in overseas emerging markets. You will take ownership of the products to ensure optimal user experience, operation efficiency, security and compliant to regulations. Responsibilities: - Play the role as a key product manager of digital wallet product which covers user acquisition, KYC / verification, top up / payment, promotion and every expects of a typical digital wallet service - Closely collaborate with strategic e-commerce platforms and other partners. Deliver and manage product solutions that help achieve business goals. - Articulate value propositions of business initiatives. Translate business requirements into product requirement that is concrete and clear for the development team to work on. - Understand competitive landscape in local markets, discover market insights and identify customer pain points - Take ownership of the product, manage short / long term product roadmap based on the business and customer value - Collaborate with different teams and stakeholders, project-manage and oversee E2E development process. - Understand user mindset and behavior through research, observation, data-analysis and E2E testing. Engineer and deliver frictionless and relevant digital wallet / payment experience to customers. - Act as an ambassador for the product internally and externally, and as the primary product contact for queries related to the product. - Understand, define and track product performance metric. Consistently iterate the products based on analysis of the product performance metric - Off-hour and on-site support to ensure product integrity during high traffic events</t>
   </si>
   <si>
     <t>- To drive partnership growth by widening network’s potential addressable base - To onboard new partners and ensure commercial success after onboarding - To assist Country Manager to manage day to day operations</t>
@@ -3190,7 +3190,7 @@
     <t>Responsible for managing the day-to-day relationship of a portfolio of Small and Medium Sized Businesses (SME) and providing a best-in-class service to ensure high conversion of new clients and excellent retention of existing clients. This is an exciting opportunity for someone with a proven record of accomplishment in managing client relationships. Key responsibilities include: Execute and trade a specific B2B portfolio working towards pre-set targets &amp; KPI’s Proactively seek out new business referrals whilst cross selling and upselling the existing portfolio into our various products, including hedging and orders Focus on deepening client relationships through active outbound and inbound calls, providing relevant market updates, leading face to face client meetings and hosting client entertainment (when Covid restrictions ease), ultimately driving client satisfaction and retention and increasing revenue in a competitive market Provide prospective and existing clients with support across online, payment and general queries as well as booking transactions over the phone resulting in an uplift in existing monthly transactions Help team member’s clients as if they were your own and ensuring they do not see a drop off in service levels when their dealer is not around Effectively manage stakeholders and build strong relationships across the business to ensure a smooth and fast e2e transaction process Proactively share knowledge, experience, concerns, and ideas with the immediate and wider dealing team to enhance the customer experience and ensure all trades are compliant and the business is protected from unnecessary risk Ensure existing and prospective clients know how to self serve through the WorldFirst platform and assist in creating a process to ensure a high % of trades are booked online Be a brand ambassador for WorldFirst - demonstrate energy, resilience and tenacity, always seeking to create solutions that exceed client expectations</t>
   </si>
   <si>
-    <t>This role will take responsibility for oversea Jurisdiction, focusing on associate with COE and dedicate for benefits strategy research, design and innovation. This includes management of and enhancements to our existing programs, and the design and implementation of new benefit programs. The scope of the role includes Global Mobility benefits, health management, supplementary pension scheme and etc. This individual contributor role will associate COE to drive employee engagement in benefits, and identify new opportunities to meet the needs of our fast growing business. Roles and Responsibilities · Benefit Strategy Research , Program Management and Design – responsible for designing benefit programs that align to Cainiao’s Global Benefits Framework, market practice and compliance requirements. This includes developing written proposals and cost impact analyses, and seeking input from a wide range of internal stakeholders to receive input and feedback on recommendations. · Implementation – responsible for implementation of approved benefit programs, including selection and setup of benefit providers, creating project plans, assembling resources, and driving employee communications. · Governance and Compliance – ensure programs align to Cainiao’s benefit philosophy and meet local regulatory requirements in all countries. This also includes monitoring costs, financial impact, future funding requirements, competitiveness, ensuring adherence with regulatory, legal and best practice approaches. · Consulting – Associate develop strategic country / jurisdiction roadmaps and provide consultative support and data-driven insights on benefit initiatives to key stakeholders including HR and Employee Relations. · Vendor Management – Manage vendor relationships, costs and performance across all countries / jurisdiction and business lines. Hold vendors to account against service levels and operate as first point of contact between Cainiao and the vendors. · Innovation – this position will drive innovation in benefits, seeking opportunities for experimentation and developing comprehensive written proposals.</t>
+    <t>This role will take responsibility for oversea Jurisdiction, focusing on associate with COE and dedicate for benefits strategy research, design and innovation. This includes management of and enhancements to our existing programs, and the design and implementation of new benefit programs. The scope of the role includes Global Mobility benefits, health management, supplementary pension scheme and etc. This individual contributor role will associate COE to drive employee engagement in benefits, and identify new opportunities to meet the needs of our fast growing business. Roles and Responsibilities - Benefit Strategy Research , Program Management and Design – responsible for designing benefit programs that align to Cainiao’s Global Benefits Framework, market practice and compliance requirements. This includes developing written proposals and cost impact analyses, and seeking input from a wide range of internal stakeholders to receive input and feedback on recommendations. - Implementation – responsible for implementation of approved benefit programs, including selection and setup of benefit providers, creating project plans, assembling resources, and driving employee communications. - Governance and Compliance – ensure programs align to Cainiao’s benefit philosophy and meet local regulatory requirements in all countries. This also includes monitoring costs, financial impact, future funding requirements, competitiveness, ensuring adherence with regulatory, legal and best practice approaches. - Consulting – Associate develop strategic country / jurisdiction roadmaps and provide consultative support and data-driven insights on benefit initiatives to key stakeholders including HR and Employee Relations. - Vendor Management – Manage vendor relationships, costs and performance across all countries / jurisdiction and business lines. Hold vendors to account against service levels and operate as first point of contact between Cainiao and the vendors. - Innovation – this position will drive innovation in benefits, seeking opportunities for experimentation and developing comprehensive written proposals.</t>
   </si>
   <si>
     <t>1、定期與其他相關部門交流預先瞭解資金需求； 2、負責銀行資金管理和投资工作，負責資金池相關數據的計量、測算及內部資金定價； 3、協助分析資產負債結構、評估及監控流動性風險及利率風險； 4、負責公司專案資金計畫及執行情況，做好專案資金的合理調配； 5、負責管理銀行日常資金管理，包括制定資金計畫、審核日常資金變動； 6、定期向資產負債管理委員會提交資金池分析報告； 7、擁有豐富的金融同業、機構客戶資源，能獨立拓展機構客戶者优先；</t>
@@ -3505,7 +3505,7 @@
     <t>- Bachelor Degree in Business, Accounting or Finance, or equivalent work experience with at least 4 to 8 years of working experience - Good knowledge of e-commerce, FINTECH, payment systems and money transmission business - Independent and self-driven, continuous breakthroughs and innovations - Knowledge of user acquisition and lifecycle management operations is highly desirable - Strong organizational and communication skills (with internal and external stakeholders), ability to break the boundary and execute to the last mile - Excellent command of spoken and written for both English and Mandarin to communicate with our Mandarin-speaking stakeholders</t>
   </si>
   <si>
-    <t>· Minimum of 3 years relevant working experience in fund management, with comprehensive financial accounting knowledge; Degree or major in accounting and finance, knowledgeable in international payment, collection and settlement business, working experience in global banks, payment companies or corporate treasury preferred · A fast learner, able to adapt to rapidly developing and changing working environment, with great teamwork and communication skills · Clear mindset and innovative, and be able to actively coordinate or lead the implementation of the responsible projects from fund management point of view · Always practice customer first and strong risk awareness on issue analysis and a comprehensive solution taking in priority and corresponding escalation when required to · Proficient in Chinese and English listening, speaking, reading and writing as the job requires to liaise with Chinese speaking counterparts</t>
+    <t>- Minimum of 3 years relevant working experience in fund management, with comprehensive financial accounting knowledge; Degree or major in accounting and finance, knowledgeable in international payment, collection and settlement business, working experience in global banks, payment companies or corporate treasury preferred - A fast learner, able to adapt to rapidly developing and changing working environment, with great teamwork and communication skills - Clear mindset and innovative, and be able to actively coordinate or lead the implementation of the responsible projects from fund management point of view - Always practice customer first and strong risk awareness on issue analysis and a comprehensive solution taking in priority and corresponding escalation when required to - Proficient in Chinese and English listening, speaking, reading and writing as the job requires to liaise with Chinese speaking counterparts</t>
   </si>
   <si>
     <t>1. . 大专及以上学历，物流管理等相关专业。 2. 具备较强的仓库现场管控能力、逻辑思维能力及基础财务知识。 3. 思维敏捷，具有较强的沟通能力和执行能力，和良好的团队意识。 4. 精通物流仓储业务并具备仓储现场运营管理经验，熟悉WMS系统。 5. 熟悉日常办公软件，熟练运用Word、Excel、PPT，具备较强的数据分析能力。 6. 具有较强的敬业精神和责任心，适应能力强，有良好的团队协作意识，擅长和人打交道，协调组织能力强。</t>
@@ -3670,7 +3670,7 @@
     <t>1. A minimum of 8 years’ relevant Compliance experience obtained in the finance or banking or Techfin industry; 2. In-depth knowledge of banking and financial and Techfin sector laws and regulations in the AML and sanctions'area is preferable; 3. Ability to understand the business, analyze issues and formulate appropriate recommendations; 4. Self-motivated, resilient, independent and able to work under pressure; 5. Excellent interpersonal and communication skills; 6. Good writing ability.</t>
   </si>
   <si>
-    <t>· 3 years and above, with experience in product management or related role. Previous experience in digital wallet, payments or eCommerce industry / O2O scenarios is highly preferred. · Good understanding on digital wallet, payment technology, payment channels and industry players in Southeast Asia markets and / or European / Brazil markets. · Hands-on experience working with both business and technical teams. Experience in understanding business requirement and defining product specifications. · Strong analytical skills and proven ability of data-driven decision-making, ability to define and manage qualitative and quantitative research and measurement plans. · Strong organizational acumen – ability to thrive in a matrix environment where success depends on a high degree of cross-functional collaboration. · Can-do attitude, willingness to learn and listen, ability to work independently, and a strong drive to get things done.</t>
+    <t>- 3 years and above, with experience in product management or related role. Previous experience in digital wallet, payments or eCommerce industry / O2O scenarios is highly preferred. - Good understanding on digital wallet, payment technology, payment channels and industry players in Southeast Asia markets and / or European / Brazil markets. - Hands-on experience working with both business and technical teams. Experience in understanding business requirement and defining product specifications. - Strong analytical skills and proven ability of data-driven decision-making, ability to define and manage qualitative and quantitative research and measurement plans. - Strong organizational acumen – ability to thrive in a matrix environment where success depends on a high degree of cross-functional collaboration. - Can-do attitude, willingness to learn and listen, ability to work independently, and a strong drive to get things done.</t>
   </si>
   <si>
     <t>- 5 years+ working experiences in payment / banking (related) industries - Financial Consultancy or investment banking experiences beneficial - Self-motivated and strong adaptability to multi-culture working environment</t>
@@ -3937,7 +3937,7 @@
     <t>Skills and experience required: Fluent in German and English Proven B2B relationship management experience Experience in financial services, e-commerce or international trade preferred but not essential Demonstrates a deep understanding of the client with a 'Customer First' mentality, possesses a keen desire to complement a strong team of excellent Relationship Managers to deliver a seamless customer experience Builds mutually beneficial relationships both internally and externally, demonstrates insightful communication skills and the confident ability to engage openly with people at all levels (including top decision makers) Keeps abreast of industry and product advancements, becomes an expert who is able to share relevant insights in a compelling and relevant manner Commercially focused and demonstrates a strong understanding of WorldFirst’s vision and mission and how you specifically create value for the business Evidences a strong track record in hitting and exceeding targets on a monthly basis providing excellent customer service, demonstrates effective time management, monitors progress and measures results against set KPI's Accountable for processes, actions and decisions under your control; consistently delivers work to the required quality and proactively suggests ways in which to improve practices and policies to the benefit of WorldFirst and its clients Ability to work under pressure and handle high workloads efficiently whilst supporting and contributing to the wider team goals Brings a positive, ‘go for it’ attitude and is real team player who is always happy to work collaboratively and will back up any role or activity needed Loves change and progress - WorldFirst clients &amp; employees will be seeing a lot of both over 2022! What we offer: Competitive salary and performance-based bonus Training and development opportunities in an international environment Dynamic team, start-up working environment in a professional organization Casual dress-code and flexibility to work from home WorldFirst is an Equal Opportunities employer, we are committed to and promote diversity and inclusivity</t>
   </si>
   <si>
-    <t>· 5+ years of experience working within employee benefits, including in-house experience. · Experience of benefit program design, development and delivery within Europe. · Ability to influence senior internal stakeholders and manage external vendors. · Ability to simplify complex topics for broad audiences. · Excellent English written and verbal communications skills - ability to interface with all levels of the organization. · Comfortable to work independently and with ambiguity to deliver the right solution for customers.</t>
+    <t>- 5+ years of experience working within employee benefits, including in-house experience. - Experience of benefit program design, development and delivery within Europe. - Ability to influence senior internal stakeholders and manage external vendors. - Ability to simplify complex topics for broad audiences. - Excellent English written and verbal communications skills - ability to interface with all levels of the organization. - Comfortable to work independently and with ambiguity to deliver the right solution for customers.</t>
   </si>
   <si>
     <t>1、學歷要求：本科及以上 2、有關工作經驗：10年以上 3、專業要求：金融專業 4、專業知識：具備資金系統知識，熟悉資金管理工作各項主要法律法規 (Basel III 和其他监管要求)，敏銳的洞察力及分析判斷能力，管理能力、溝通及協調技巧以及承受壓力的能力 5、語文要求：有較好的中英語讀、寫能力</t>

</xml_diff>